<commit_message>
Limpieza y insights completos
</commit_message>
<xml_diff>
--- a/AquaVentura.xlsx
+++ b/AquaVentura.xlsx
@@ -509,7 +509,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -562,7 +562,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -615,7 +615,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -668,7 +668,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -774,7 +774,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -827,7 +827,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -880,7 +880,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -933,7 +933,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -954,7 +954,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -982,7 +982,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1035,7 +1035,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1084,7 +1084,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1133,7 +1133,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1186,7 +1186,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1239,7 +1239,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1292,7 +1292,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1345,7 +1345,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1394,7 +1394,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1447,7 +1447,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1500,7 +1500,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1659,7 +1659,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1712,7 +1712,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1765,7 +1765,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1818,7 +1818,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1867,7 +1867,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1920,7 +1920,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1969,7 +1969,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2022,7 +2022,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2075,7 +2075,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2124,7 +2124,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2173,7 +2173,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2226,7 +2226,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2279,7 +2279,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2332,7 +2332,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2410,7 +2410,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -2438,7 +2438,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2487,7 +2487,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2593,7 +2593,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2646,7 +2646,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2699,7 +2699,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2748,7 +2748,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2801,7 +2801,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2822,7 +2822,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -2850,7 +2850,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2860,7 +2860,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H47" t="inlineStr"/>
@@ -2871,7 +2871,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -2899,7 +2899,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2952,7 +2952,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -3005,7 +3005,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -3058,7 +3058,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -3111,7 +3111,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -3164,7 +3164,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -3217,7 +3217,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -3242,7 +3242,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -3270,7 +3270,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -3323,7 +3323,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -3333,7 +3333,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H56" t="inlineStr"/>
@@ -3372,7 +3372,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -3421,7 +3421,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -3470,7 +3470,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -3523,7 +3523,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -3576,7 +3576,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -3586,7 +3586,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H61" t="inlineStr"/>
@@ -3625,7 +3625,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -3678,7 +3678,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -3731,7 +3731,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -3780,7 +3780,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -3833,7 +3833,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -3886,7 +3886,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -3939,7 +3939,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -3992,7 +3992,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -4002,7 +4002,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -4017,7 +4017,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -4045,7 +4045,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -4098,7 +4098,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -4151,7 +4151,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -4204,7 +4204,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -4253,7 +4253,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -4302,7 +4302,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -4355,7 +4355,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -4404,7 +4404,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -4457,7 +4457,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -4510,7 +4510,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -4563,7 +4563,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -4612,7 +4612,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -4661,7 +4661,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -4710,7 +4710,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -4763,7 +4763,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -4788,7 +4788,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -4816,7 +4816,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -4869,7 +4869,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -4922,7 +4922,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -4975,7 +4975,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -4985,7 +4985,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H88" t="inlineStr"/>
@@ -5024,7 +5024,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -5073,7 +5073,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -5126,7 +5126,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -5179,7 +5179,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -5232,7 +5232,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -5285,7 +5285,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -5391,7 +5391,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -5416,7 +5416,7 @@
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
@@ -5444,7 +5444,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -5465,7 +5465,7 @@
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K97" t="inlineStr">
@@ -5493,7 +5493,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -5546,7 +5546,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -5567,7 +5567,7 @@
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K99" t="inlineStr">
@@ -5595,7 +5595,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -5644,7 +5644,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -5654,7 +5654,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H101" t="inlineStr"/>
@@ -5693,7 +5693,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -5718,7 +5718,7 @@
       </c>
       <c r="J102" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K102" t="inlineStr">
@@ -5746,7 +5746,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -5799,7 +5799,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -5848,7 +5848,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -5901,7 +5901,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -5954,7 +5954,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -6007,7 +6007,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -6017,7 +6017,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H108" t="inlineStr"/>
@@ -6056,7 +6056,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -6066,7 +6066,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H109" t="inlineStr"/>
@@ -6077,7 +6077,7 @@
       </c>
       <c r="J109" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K109" t="inlineStr">
@@ -6105,7 +6105,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -6158,7 +6158,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -6211,7 +6211,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -6264,7 +6264,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -6317,7 +6317,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -6370,7 +6370,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -6423,7 +6423,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -6476,7 +6476,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -6529,7 +6529,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -6554,7 +6554,7 @@
       </c>
       <c r="J118" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K118" t="inlineStr">
@@ -6582,7 +6582,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -6635,7 +6635,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -6688,7 +6688,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -6737,7 +6737,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -6790,7 +6790,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -6843,7 +6843,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -6853,7 +6853,7 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H124" t="inlineStr"/>
@@ -6892,7 +6892,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -6945,7 +6945,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -6998,7 +6998,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -7008,7 +7008,7 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H127" t="inlineStr"/>
@@ -7047,7 +7047,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -7057,7 +7057,7 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H128" t="inlineStr"/>
@@ -7096,7 +7096,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -7145,7 +7145,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -7198,7 +7198,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -7208,7 +7208,7 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H131" t="inlineStr"/>
@@ -7247,7 +7247,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -7296,7 +7296,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -7345,7 +7345,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -7355,7 +7355,7 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H134" t="inlineStr"/>
@@ -7366,7 +7366,7 @@
       </c>
       <c r="J134" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K134" t="inlineStr">
@@ -7394,7 +7394,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -7415,7 +7415,7 @@
       </c>
       <c r="J135" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K135" t="inlineStr">
@@ -7443,7 +7443,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -7453,7 +7453,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H136" t="inlineStr"/>
@@ -7492,7 +7492,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -7541,7 +7541,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -7551,7 +7551,7 @@
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H138" t="inlineStr"/>
@@ -7590,7 +7590,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -7639,7 +7639,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -7688,7 +7688,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -7737,7 +7737,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -7786,7 +7786,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -7811,7 +7811,7 @@
       </c>
       <c r="J143" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K143" t="inlineStr">
@@ -7839,7 +7839,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -7888,7 +7888,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -7937,7 +7937,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -7986,7 +7986,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -8039,7 +8039,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -8088,7 +8088,7 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -8098,7 +8098,7 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H149" t="inlineStr"/>
@@ -8137,7 +8137,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -8190,7 +8190,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -8239,7 +8239,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -8260,7 +8260,7 @@
       </c>
       <c r="J152" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K152" t="inlineStr">
@@ -8288,7 +8288,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -8341,7 +8341,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -8390,7 +8390,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -8439,7 +8439,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -8492,7 +8492,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -8502,7 +8502,7 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H157" t="inlineStr"/>
@@ -8541,7 +8541,7 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -8594,7 +8594,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -8647,7 +8647,7 @@
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -8700,7 +8700,7 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -8753,7 +8753,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -8763,7 +8763,7 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H162" t="inlineStr">
@@ -8806,7 +8806,7 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -8859,7 +8859,7 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -8912,7 +8912,7 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -8965,7 +8965,7 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -8986,7 +8986,7 @@
       </c>
       <c r="J166" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K166" t="inlineStr">
@@ -9014,7 +9014,7 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -9024,7 +9024,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H167" t="inlineStr"/>
@@ -9063,7 +9063,7 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -9116,7 +9116,7 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -9165,7 +9165,7 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -9186,7 +9186,7 @@
       </c>
       <c r="J170" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K170" t="inlineStr">
@@ -9214,7 +9214,7 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -9224,7 +9224,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H171" t="inlineStr"/>
@@ -9263,7 +9263,7 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -9288,7 +9288,7 @@
       </c>
       <c r="J172" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K172" t="inlineStr">
@@ -9316,7 +9316,7 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -9326,7 +9326,7 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H173" t="inlineStr"/>
@@ -9365,7 +9365,7 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -9375,7 +9375,7 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H174" t="inlineStr"/>
@@ -9414,7 +9414,7 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -9467,7 +9467,7 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -9516,7 +9516,7 @@
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -9526,7 +9526,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H177" t="inlineStr">
@@ -9541,7 +9541,7 @@
       </c>
       <c r="J177" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K177" t="inlineStr">
@@ -9569,7 +9569,7 @@
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -9622,7 +9622,7 @@
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -9671,7 +9671,7 @@
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
@@ -9681,7 +9681,7 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H180" t="inlineStr"/>
@@ -9720,7 +9720,7 @@
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
@@ -9773,7 +9773,7 @@
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -9794,7 +9794,7 @@
       </c>
       <c r="J182" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K182" t="inlineStr">
@@ -9822,7 +9822,7 @@
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -9875,7 +9875,7 @@
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
@@ -9928,7 +9928,7 @@
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
@@ -9977,7 +9977,7 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -10026,7 +10026,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
@@ -10079,7 +10079,7 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -10132,7 +10132,7 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -10185,7 +10185,7 @@
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -10238,7 +10238,7 @@
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -10248,7 +10248,7 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H191" t="inlineStr"/>
@@ -10287,7 +10287,7 @@
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
@@ -10340,7 +10340,7 @@
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -10393,7 +10393,7 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -10403,7 +10403,7 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H194" t="inlineStr"/>
@@ -10414,7 +10414,7 @@
       </c>
       <c r="J194" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K194" t="inlineStr">
@@ -10442,7 +10442,7 @@
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -10491,7 +10491,7 @@
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -10501,7 +10501,7 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H196" t="inlineStr"/>
@@ -10540,7 +10540,7 @@
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -10550,7 +10550,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H197" t="inlineStr"/>
@@ -10561,7 +10561,7 @@
       </c>
       <c r="J197" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K197" t="inlineStr">
@@ -10589,7 +10589,7 @@
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -10638,7 +10638,7 @@
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
@@ -10691,7 +10691,7 @@
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
@@ -10744,7 +10744,7 @@
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -10793,7 +10793,7 @@
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -10842,7 +10842,7 @@
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -10895,7 +10895,7 @@
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -10944,7 +10944,7 @@
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -10954,7 +10954,7 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H205" t="inlineStr"/>
@@ -10993,7 +10993,7 @@
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -11018,7 +11018,7 @@
       </c>
       <c r="J206" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K206" t="inlineStr">
@@ -11046,7 +11046,7 @@
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -11071,7 +11071,7 @@
       </c>
       <c r="J207" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K207" t="inlineStr">
@@ -11099,7 +11099,7 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -11109,7 +11109,7 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H208" t="inlineStr"/>
@@ -11148,7 +11148,7 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -11197,7 +11197,7 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -11250,7 +11250,7 @@
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -11303,7 +11303,7 @@
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -11352,7 +11352,7 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -11401,7 +11401,7 @@
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -11454,7 +11454,7 @@
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -11503,7 +11503,7 @@
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -11513,7 +11513,7 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H216" t="inlineStr"/>
@@ -11552,7 +11552,7 @@
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -11601,7 +11601,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -11650,7 +11650,7 @@
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -11675,7 +11675,7 @@
       </c>
       <c r="J219" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K219" t="inlineStr">
@@ -11703,7 +11703,7 @@
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -11713,7 +11713,7 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H220" t="inlineStr"/>
@@ -11724,7 +11724,7 @@
       </c>
       <c r="J220" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K220" t="inlineStr">
@@ -11752,7 +11752,7 @@
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -11762,7 +11762,7 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H221" t="inlineStr">
@@ -11777,7 +11777,7 @@
       </c>
       <c r="J221" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K221" t="inlineStr">
@@ -11805,7 +11805,7 @@
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -11815,7 +11815,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H222" t="inlineStr"/>
@@ -11854,7 +11854,7 @@
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -11907,7 +11907,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -11960,7 +11960,7 @@
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -12013,7 +12013,7 @@
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -12066,7 +12066,7 @@
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -12115,7 +12115,7 @@
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -12168,7 +12168,7 @@
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -12221,7 +12221,7 @@
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -12270,7 +12270,7 @@
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
@@ -12280,7 +12280,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H231" t="inlineStr"/>
@@ -12291,7 +12291,7 @@
       </c>
       <c r="J231" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K231" t="inlineStr">
@@ -12319,7 +12319,7 @@
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -12344,7 +12344,7 @@
       </c>
       <c r="J232" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K232" t="inlineStr">
@@ -12372,7 +12372,7 @@
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -12421,7 +12421,7 @@
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -12470,7 +12470,7 @@
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -12519,7 +12519,7 @@
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -12529,7 +12529,7 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H236" t="inlineStr"/>
@@ -12540,7 +12540,7 @@
       </c>
       <c r="J236" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K236" t="inlineStr">
@@ -12568,7 +12568,7 @@
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
@@ -12617,7 +12617,7 @@
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -12670,7 +12670,7 @@
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
@@ -12695,7 +12695,7 @@
       </c>
       <c r="J239" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K239" t="inlineStr">
@@ -12723,7 +12723,7 @@
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -12776,7 +12776,7 @@
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -12825,7 +12825,7 @@
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -12878,7 +12878,7 @@
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -12931,7 +12931,7 @@
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
@@ -12984,7 +12984,7 @@
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
@@ -13037,7 +13037,7 @@
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
@@ -13090,7 +13090,7 @@
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
@@ -13143,7 +13143,7 @@
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F248" t="inlineStr">
@@ -13153,7 +13153,7 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H248" t="inlineStr"/>
@@ -13192,7 +13192,7 @@
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F249" t="inlineStr">
@@ -13241,7 +13241,7 @@
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F250" t="inlineStr">
@@ -13294,7 +13294,7 @@
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
@@ -13347,7 +13347,7 @@
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
@@ -13368,7 +13368,7 @@
       </c>
       <c r="J252" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K252" t="inlineStr">
@@ -13396,7 +13396,7 @@
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F253" t="inlineStr">
@@ -13449,7 +13449,7 @@
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F254" t="inlineStr">
@@ -13498,7 +13498,7 @@
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F255" t="inlineStr">
@@ -13508,7 +13508,7 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H255" t="inlineStr"/>
@@ -13547,7 +13547,7 @@
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
@@ -13557,7 +13557,7 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H256" t="inlineStr"/>
@@ -13596,7 +13596,7 @@
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
@@ -13645,7 +13645,7 @@
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F258" t="inlineStr">
@@ -13698,7 +13698,7 @@
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F259" t="inlineStr">
@@ -13747,7 +13747,7 @@
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -13796,7 +13796,7 @@
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -13845,7 +13845,7 @@
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
@@ -13894,7 +13894,7 @@
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
@@ -13904,7 +13904,7 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H263" t="inlineStr"/>
@@ -13943,7 +13943,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
@@ -13968,7 +13968,7 @@
       </c>
       <c r="J264" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K264" t="inlineStr">
@@ -13996,7 +13996,7 @@
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
@@ -14006,7 +14006,7 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H265" t="inlineStr"/>
@@ -14045,7 +14045,7 @@
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -14094,7 +14094,7 @@
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
@@ -14143,7 +14143,7 @@
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
@@ -14192,7 +14192,7 @@
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
@@ -14241,7 +14241,7 @@
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -14251,7 +14251,7 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H270" t="inlineStr"/>
@@ -14290,7 +14290,7 @@
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -14343,7 +14343,7 @@
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
@@ -14396,7 +14396,7 @@
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
@@ -14445,7 +14445,7 @@
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
@@ -14494,7 +14494,7 @@
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
@@ -14504,7 +14504,7 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H275" t="inlineStr"/>
@@ -14515,7 +14515,7 @@
       </c>
       <c r="J275" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K275" t="inlineStr">
@@ -14543,7 +14543,7 @@
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -14592,7 +14592,7 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -14641,7 +14641,7 @@
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -14690,7 +14690,7 @@
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
@@ -14743,7 +14743,7 @@
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
@@ -14796,7 +14796,7 @@
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
@@ -14849,7 +14849,7 @@
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -14898,7 +14898,7 @@
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
@@ -14908,7 +14908,7 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H283" t="inlineStr"/>
@@ -14947,7 +14947,7 @@
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
@@ -15000,7 +15000,7 @@
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -15053,7 +15053,7 @@
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -15063,7 +15063,7 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H286" t="inlineStr"/>
@@ -15102,7 +15102,7 @@
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -15155,7 +15155,7 @@
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
@@ -15204,7 +15204,7 @@
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -15253,7 +15253,7 @@
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
@@ -15302,7 +15302,7 @@
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
@@ -15312,7 +15312,7 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H291" t="inlineStr"/>
@@ -15351,7 +15351,7 @@
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -15372,7 +15372,7 @@
       </c>
       <c r="J292" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K292" t="inlineStr">
@@ -15400,7 +15400,7 @@
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -15449,7 +15449,7 @@
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -15498,7 +15498,7 @@
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
@@ -15508,7 +15508,7 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H295" t="inlineStr"/>
@@ -15547,7 +15547,7 @@
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
@@ -15557,7 +15557,7 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H296" t="inlineStr"/>
@@ -15596,7 +15596,7 @@
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
@@ -15617,7 +15617,7 @@
       </c>
       <c r="J297" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K297" t="inlineStr">
@@ -15645,7 +15645,7 @@
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
@@ -15694,7 +15694,7 @@
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -15747,7 +15747,7 @@
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -15796,7 +15796,7 @@
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
@@ -15806,7 +15806,7 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H301" t="inlineStr"/>
@@ -15817,7 +15817,7 @@
       </c>
       <c r="J301" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K301" t="inlineStr">
@@ -15845,7 +15845,7 @@
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
@@ -15894,7 +15894,7 @@
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
@@ -15943,7 +15943,7 @@
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
@@ -15992,7 +15992,7 @@
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
@@ -16041,7 +16041,7 @@
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -16090,7 +16090,7 @@
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
@@ -16139,7 +16139,7 @@
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
@@ -16188,7 +16188,7 @@
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -16237,7 +16237,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
@@ -16286,7 +16286,7 @@
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
@@ -16335,7 +16335,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -16388,7 +16388,7 @@
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -16437,7 +16437,7 @@
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
@@ -16486,7 +16486,7 @@
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
@@ -16507,7 +16507,7 @@
       </c>
       <c r="J315" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K315" t="inlineStr">
@@ -16535,7 +16535,7 @@
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
@@ -16584,7 +16584,7 @@
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
@@ -16605,7 +16605,7 @@
       </c>
       <c r="J317" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K317" t="inlineStr">
@@ -16633,7 +16633,7 @@
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
@@ -16643,7 +16643,7 @@
       </c>
       <c r="G318" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H318" t="inlineStr"/>
@@ -16682,7 +16682,7 @@
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
@@ -16731,7 +16731,7 @@
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
@@ -16780,7 +16780,7 @@
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
@@ -16829,7 +16829,7 @@
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
@@ -16878,7 +16878,7 @@
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
@@ -16888,7 +16888,7 @@
       </c>
       <c r="G323" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H323" t="inlineStr"/>
@@ -16899,7 +16899,7 @@
       </c>
       <c r="J323" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K323" t="inlineStr">
@@ -16927,7 +16927,7 @@
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
@@ -16976,7 +16976,7 @@
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
@@ -17025,7 +17025,7 @@
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
@@ -17074,7 +17074,7 @@
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
@@ -17123,7 +17123,7 @@
       </c>
       <c r="E328" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F328" t="inlineStr">
@@ -17172,7 +17172,7 @@
       </c>
       <c r="E329" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F329" t="inlineStr">
@@ -17221,7 +17221,7 @@
       </c>
       <c r="E330" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F330" t="inlineStr">
@@ -17270,7 +17270,7 @@
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F331" t="inlineStr">
@@ -17319,7 +17319,7 @@
       </c>
       <c r="E332" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F332" t="inlineStr">
@@ -17368,7 +17368,7 @@
       </c>
       <c r="E333" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F333" t="inlineStr">
@@ -17417,7 +17417,7 @@
       </c>
       <c r="E334" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F334" t="inlineStr">
@@ -17466,7 +17466,7 @@
       </c>
       <c r="E335" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F335" t="inlineStr">
@@ -17515,7 +17515,7 @@
       </c>
       <c r="E336" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F336" t="inlineStr">
@@ -17568,7 +17568,7 @@
       </c>
       <c r="E337" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F337" t="inlineStr">
@@ -17617,7 +17617,7 @@
       </c>
       <c r="E338" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F338" t="inlineStr">
@@ -17666,7 +17666,7 @@
       </c>
       <c r="E339" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F339" t="inlineStr">
@@ -17715,7 +17715,7 @@
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F340" t="inlineStr">
@@ -17764,7 +17764,7 @@
       </c>
       <c r="E341" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F341" t="inlineStr">
@@ -17813,7 +17813,7 @@
       </c>
       <c r="E342" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F342" t="inlineStr">
@@ -17862,7 +17862,7 @@
       </c>
       <c r="E343" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F343" t="inlineStr">
@@ -17911,7 +17911,7 @@
       </c>
       <c r="E344" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F344" t="inlineStr">
@@ -17960,7 +17960,7 @@
       </c>
       <c r="E345" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F345" t="inlineStr">
@@ -18009,7 +18009,7 @@
       </c>
       <c r="E346" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F346" t="inlineStr">
@@ -18058,7 +18058,7 @@
       </c>
       <c r="E347" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F347" t="inlineStr">
@@ -18107,7 +18107,7 @@
       </c>
       <c r="E348" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F348" t="inlineStr">
@@ -18156,7 +18156,7 @@
       </c>
       <c r="E349" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F349" t="inlineStr">
@@ -18205,7 +18205,7 @@
       </c>
       <c r="E350" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F350" t="inlineStr">
@@ -18215,7 +18215,7 @@
       </c>
       <c r="G350" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H350" t="inlineStr"/>
@@ -18254,7 +18254,7 @@
       </c>
       <c r="E351" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F351" t="inlineStr">
@@ -18303,7 +18303,7 @@
       </c>
       <c r="E352" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F352" t="inlineStr">
@@ -18324,7 +18324,7 @@
       </c>
       <c r="J352" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K352" t="inlineStr">
@@ -18352,7 +18352,7 @@
       </c>
       <c r="E353" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F353" t="inlineStr">
@@ -18401,7 +18401,7 @@
       </c>
       <c r="E354" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F354" t="inlineStr">
@@ -18422,7 +18422,7 @@
       </c>
       <c r="J354" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K354" t="inlineStr">
@@ -18450,7 +18450,7 @@
       </c>
       <c r="E355" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F355" t="inlineStr">
@@ -18499,7 +18499,7 @@
       </c>
       <c r="E356" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F356" t="inlineStr">
@@ -18548,7 +18548,7 @@
       </c>
       <c r="E357" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F357" t="inlineStr">
@@ -18569,7 +18569,7 @@
       </c>
       <c r="J357" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K357" t="inlineStr">
@@ -18597,7 +18597,7 @@
       </c>
       <c r="E358" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F358" t="inlineStr">
@@ -18618,7 +18618,7 @@
       </c>
       <c r="J358" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K358" t="inlineStr">
@@ -18646,7 +18646,7 @@
       </c>
       <c r="E359" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F359" t="inlineStr">
@@ -18695,7 +18695,7 @@
       </c>
       <c r="E360" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F360" t="inlineStr">
@@ -18744,7 +18744,7 @@
       </c>
       <c r="E361" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F361" t="inlineStr">
@@ -18793,7 +18793,7 @@
       </c>
       <c r="E362" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F362" t="inlineStr">
@@ -18803,7 +18803,7 @@
       </c>
       <c r="G362" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H362" t="inlineStr"/>
@@ -18814,7 +18814,7 @@
       </c>
       <c r="J362" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K362" t="inlineStr">
@@ -18842,7 +18842,7 @@
       </c>
       <c r="E363" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F363" t="inlineStr">
@@ -18891,7 +18891,7 @@
       </c>
       <c r="E364" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F364" t="inlineStr">
@@ -18940,7 +18940,7 @@
       </c>
       <c r="E365" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F365" t="inlineStr">
@@ -18989,7 +18989,7 @@
       </c>
       <c r="E366" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F366" t="inlineStr">
@@ -19038,7 +19038,7 @@
       </c>
       <c r="E367" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F367" t="inlineStr">
@@ -19048,7 +19048,7 @@
       </c>
       <c r="G367" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H367" t="inlineStr"/>
@@ -19059,7 +19059,7 @@
       </c>
       <c r="J367" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K367" t="inlineStr">
@@ -19087,7 +19087,7 @@
       </c>
       <c r="E368" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F368" t="inlineStr">
@@ -19097,7 +19097,7 @@
       </c>
       <c r="G368" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H368" t="inlineStr"/>
@@ -19136,7 +19136,7 @@
       </c>
       <c r="E369" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F369" t="inlineStr">
@@ -19146,7 +19146,7 @@
       </c>
       <c r="G369" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H369" t="inlineStr"/>
@@ -19157,7 +19157,7 @@
       </c>
       <c r="J369" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K369" t="inlineStr">
@@ -19185,7 +19185,7 @@
       </c>
       <c r="E370" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F370" t="inlineStr">
@@ -19195,7 +19195,7 @@
       </c>
       <c r="G370" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H370" t="inlineStr"/>
@@ -19206,7 +19206,7 @@
       </c>
       <c r="J370" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K370" t="inlineStr">
@@ -19234,7 +19234,7 @@
       </c>
       <c r="E371" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F371" t="inlineStr">
@@ -19283,7 +19283,7 @@
       </c>
       <c r="E372" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F372" t="inlineStr">
@@ -19304,7 +19304,7 @@
       </c>
       <c r="J372" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K372" t="inlineStr">
@@ -19332,7 +19332,7 @@
       </c>
       <c r="E373" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F373" t="inlineStr">
@@ -19342,7 +19342,7 @@
       </c>
       <c r="G373" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H373" t="inlineStr"/>
@@ -19381,7 +19381,7 @@
       </c>
       <c r="E374" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F374" t="inlineStr">
@@ -19434,7 +19434,7 @@
       </c>
       <c r="E375" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F375" t="inlineStr">
@@ -19483,7 +19483,7 @@
       </c>
       <c r="E376" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F376" t="inlineStr">
@@ -19532,7 +19532,7 @@
       </c>
       <c r="E377" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F377" t="inlineStr">
@@ -19542,7 +19542,7 @@
       </c>
       <c r="G377" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H377" t="inlineStr"/>
@@ -19581,7 +19581,7 @@
       </c>
       <c r="E378" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F378" t="inlineStr">
@@ -19630,7 +19630,7 @@
       </c>
       <c r="E379" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F379" t="inlineStr">
@@ -19683,7 +19683,7 @@
       </c>
       <c r="E380" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F380" t="inlineStr">
@@ -19704,7 +19704,7 @@
       </c>
       <c r="J380" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K380" t="inlineStr">
@@ -19732,7 +19732,7 @@
       </c>
       <c r="E381" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F381" t="inlineStr">
@@ -19753,7 +19753,7 @@
       </c>
       <c r="J381" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K381" t="inlineStr">
@@ -19781,7 +19781,7 @@
       </c>
       <c r="E382" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F382" t="inlineStr">
@@ -19830,7 +19830,7 @@
       </c>
       <c r="E383" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F383" t="inlineStr">
@@ -19879,7 +19879,7 @@
       </c>
       <c r="E384" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F384" t="inlineStr">
@@ -19928,7 +19928,7 @@
       </c>
       <c r="E385" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F385" t="inlineStr">
@@ -19977,7 +19977,7 @@
       </c>
       <c r="E386" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F386" t="inlineStr">
@@ -20026,7 +20026,7 @@
       </c>
       <c r="E387" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F387" t="inlineStr">
@@ -20075,7 +20075,7 @@
       </c>
       <c r="E388" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F388" t="inlineStr">
@@ -20124,7 +20124,7 @@
       </c>
       <c r="E389" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F389" t="inlineStr">
@@ -20145,7 +20145,7 @@
       </c>
       <c r="J389" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K389" t="inlineStr">
@@ -20173,7 +20173,7 @@
       </c>
       <c r="E390" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F390" t="inlineStr">
@@ -20226,7 +20226,7 @@
       </c>
       <c r="E391" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F391" t="inlineStr">
@@ -20279,7 +20279,7 @@
       </c>
       <c r="E392" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F392" t="inlineStr">
@@ -20328,7 +20328,7 @@
       </c>
       <c r="E393" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F393" t="inlineStr">
@@ -20377,7 +20377,7 @@
       </c>
       <c r="E394" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F394" t="inlineStr">
@@ -20426,7 +20426,7 @@
       </c>
       <c r="E395" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F395" t="inlineStr">
@@ -20475,7 +20475,7 @@
       </c>
       <c r="E396" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F396" t="inlineStr">
@@ -20524,7 +20524,7 @@
       </c>
       <c r="E397" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F397" t="inlineStr">
@@ -20573,7 +20573,7 @@
       </c>
       <c r="E398" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F398" t="inlineStr">
@@ -20626,7 +20626,7 @@
       </c>
       <c r="E399" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F399" t="inlineStr">
@@ -20636,7 +20636,7 @@
       </c>
       <c r="G399" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H399" t="inlineStr"/>
@@ -20675,7 +20675,7 @@
       </c>
       <c r="E400" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F400" t="inlineStr">
@@ -20724,7 +20724,7 @@
       </c>
       <c r="E401" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F401" t="inlineStr">
@@ -20773,7 +20773,7 @@
       </c>
       <c r="E402" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F402" t="inlineStr">
@@ -20822,7 +20822,7 @@
       </c>
       <c r="E403" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F403" t="inlineStr">
@@ -20871,7 +20871,7 @@
       </c>
       <c r="E404" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F404" t="inlineStr">
@@ -20881,7 +20881,7 @@
       </c>
       <c r="G404" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H404" t="inlineStr"/>
@@ -20892,7 +20892,7 @@
       </c>
       <c r="J404" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K404" t="inlineStr">
@@ -20920,7 +20920,7 @@
       </c>
       <c r="E405" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F405" t="inlineStr">
@@ -20969,7 +20969,7 @@
       </c>
       <c r="E406" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F406" t="inlineStr">
@@ -20990,7 +20990,7 @@
       </c>
       <c r="J406" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="K406" t="inlineStr">
@@ -21018,7 +21018,7 @@
       </c>
       <c r="E407" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F407" t="inlineStr">
@@ -21067,7 +21067,7 @@
       </c>
       <c r="E408" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F408" t="inlineStr">
@@ -21120,7 +21120,7 @@
       </c>
       <c r="E409" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F409" t="inlineStr">
@@ -21169,7 +21169,7 @@
       </c>
       <c r="E410" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F410" t="inlineStr">
@@ -21218,7 +21218,7 @@
       </c>
       <c r="E411" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F411" t="inlineStr">
@@ -21267,7 +21267,7 @@
       </c>
       <c r="E412" t="inlineStr">
         <is>
-          <t>Watercraft</t>
+          <t>watercraft</t>
         </is>
       </c>
       <c r="F412" t="inlineStr">
@@ -21316,7 +21316,7 @@
       </c>
       <c r="E413" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F413" t="inlineStr">
@@ -21365,7 +21365,7 @@
       </c>
       <c r="E414" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="F414" t="inlineStr">
@@ -21418,7 +21418,7 @@
       </c>
       <c r="E415" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F415" t="inlineStr">
@@ -21428,7 +21428,7 @@
       </c>
       <c r="G415" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="H415" t="inlineStr"/>
@@ -21467,7 +21467,7 @@
       </c>
       <c r="E416" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F416" t="inlineStr">
@@ -21516,7 +21516,7 @@
       </c>
       <c r="E417" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F417" t="inlineStr">
@@ -21565,7 +21565,7 @@
       </c>
       <c r="E418" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F418" t="inlineStr">
@@ -21614,7 +21614,7 @@
       </c>
       <c r="E419" t="inlineStr">
         <is>
-          <t>Provoked</t>
+          <t>provoked</t>
         </is>
       </c>
       <c r="F419" t="inlineStr">
@@ -21667,7 +21667,7 @@
       </c>
       <c r="E420" t="inlineStr">
         <is>
-          <t>Unprovoked</t>
+          <t>unprovoked</t>
         </is>
       </c>
       <c r="F420" t="inlineStr">

</xml_diff>